<commit_message>
Continuing to build out character creator
</commit_message>
<xml_diff>
--- a/data/character/races.xlsx
+++ b/data/character/races.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="195">
   <si>
     <t xml:space="preserve">RACE</t>
   </si>
@@ -52,6 +52,9 @@
     <t xml:space="preserve">CHA</t>
   </si>
   <si>
+    <t xml:space="preserve">SPECIAL</t>
+  </si>
+  <si>
     <t xml:space="preserve">LANGUAGES</t>
   </si>
   <si>
@@ -277,7 +280,7 @@
     <t xml:space="preserve">Water</t>
   </si>
   <si>
-    <t xml:space="preserve">30S</t>
+    <t xml:space="preserve">30/30S</t>
   </si>
   <si>
     <t xml:space="preserve">Acid resistance, Amphibious, Swim, Call to the Wave</t>
@@ -502,9 +505,6 @@
     <t xml:space="preserve">Lizardfolk</t>
   </si>
   <si>
-    <t xml:space="preserve">30/30S</t>
-  </si>
-  <si>
     <t xml:space="preserve">Common and Draconic</t>
   </si>
   <si>
@@ -562,7 +562,7 @@
     <t xml:space="preserve">Winged</t>
   </si>
   <si>
-    <t xml:space="preserve">30F</t>
+    <t xml:space="preserve">30/30F</t>
   </si>
   <si>
     <t xml:space="preserve">Replace Hellish Rebuke with Burning Hands</t>
@@ -620,6 +620,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -722,12 +723,12 @@
   <dimension ref="A1:N57"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G18" activeCellId="0" sqref="G18"/>
+      <selection pane="topLeft" activeCell="M1" activeCellId="0" sqref="C1:M1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="17.9" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="17.9" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="3.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="7.12"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -761,60 +762,62 @@
       <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2"/>
+      <c r="K1" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="L1" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E2" s="2"/>
       <c r="F2" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
       <c r="I2" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
       <c r="L2" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D3" s="1" t="n">
         <v>30</v>
@@ -827,117 +830,129 @@
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
       <c r="L3" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
+        <v>26</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="1" t="n">
+        <v>30</v>
+      </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
       <c r="I4" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
       <c r="M4" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
+        <v>29</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="1" t="n">
+        <v>30</v>
+      </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
       <c r="G5" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
       <c r="J5" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="K5" s="2"/>
       <c r="L5" s="2"/>
       <c r="M5" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
+        <v>32</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="1" t="n">
+        <v>30</v>
+      </c>
       <c r="E6" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
       <c r="J6" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
       <c r="M6" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D7" s="1" t="n">
         <v>30</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
@@ -945,58 +960,58 @@
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
       <c r="L7" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D8" s="1" t="n">
         <v>30</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
       <c r="J8" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="K8" s="2"/>
       <c r="L8" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D9" s="1" t="n">
         <v>25</v>
@@ -1009,58 +1024,66 @@
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
       <c r="L9" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
+        <v>46</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" s="1" t="n">
+        <v>25</v>
+      </c>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
       <c r="G10" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H10" s="2"/>
       <c r="I10" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
       <c r="L10" s="2"/>
       <c r="M10" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
+        <v>49</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="1" t="n">
+        <v>25</v>
+      </c>
       <c r="E11" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
@@ -1068,51 +1091,55 @@
       <c r="K11" s="2"/>
       <c r="L11" s="2"/>
       <c r="M11" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
+        <v>51</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" s="1" t="n">
+        <v>25</v>
+      </c>
       <c r="E12" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F12" s="2"/>
       <c r="G12" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
       <c r="L12" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D13" s="1" t="n">
         <v>30</v>
@@ -1125,57 +1152,65 @@
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
       <c r="L13" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="M13" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="N13" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
+        <v>59</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" s="1" t="n">
+        <v>30</v>
+      </c>
       <c r="E14" s="2"/>
       <c r="F14" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G14" s="2"/>
       <c r="H14" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
       <c r="L14" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="M14" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="N14" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
+        <v>63</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D15" s="1" t="n">
+        <v>30</v>
+      </c>
       <c r="E15" s="2"/>
       <c r="F15" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
@@ -1184,113 +1219,121 @@
       <c r="K15" s="2"/>
       <c r="L15" s="2"/>
       <c r="M15" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="N15" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
+        <v>66</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16" s="1" t="n">
+        <v>30</v>
+      </c>
       <c r="E16" s="2"/>
       <c r="F16" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
       <c r="J16" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="K16" s="2"/>
       <c r="L16" s="2"/>
       <c r="M16" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="N16" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
+        <v>68</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D17" s="1" t="n">
+        <v>30</v>
+      </c>
       <c r="E17" s="2"/>
       <c r="F17" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G17" s="2"/>
       <c r="H17" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
       <c r="L17" s="2"/>
       <c r="M17" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="N17" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D18" s="1" t="n">
         <v>30</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
       <c r="I18" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J18" s="2"/>
       <c r="K18" s="2"/>
       <c r="L18" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="M18" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="N18" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D19" s="1" t="n">
         <v>30</v>
@@ -1303,28 +1346,32 @@
       <c r="J19" s="2"/>
       <c r="K19" s="2"/>
       <c r="L19" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="M19" s="2"/>
       <c r="N19" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
+        <v>78</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D20" s="1" t="n">
+        <v>30</v>
+      </c>
       <c r="E20" s="2"/>
       <c r="F20" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
@@ -1332,27 +1379,31 @@
       <c r="K20" s="2"/>
       <c r="L20" s="2"/>
       <c r="M20" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="N20" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
+        <v>81</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D21" s="1" t="n">
+        <v>30</v>
+      </c>
       <c r="E21" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F21" s="2"/>
       <c r="G21" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
@@ -1360,79 +1411,85 @@
       <c r="K21" s="2"/>
       <c r="L21" s="2"/>
       <c r="M21" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="N21" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
+        <v>83</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D22" s="1" t="n">
+        <v>30</v>
+      </c>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
       <c r="G22" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
       <c r="K22" s="2"/>
       <c r="L22" s="2"/>
       <c r="M22" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="N22" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="C23" s="2"/>
+        <v>85</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>15</v>
+      </c>
       <c r="D23" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
       <c r="G23" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H23" s="2"/>
       <c r="I23" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J23" s="2"/>
       <c r="K23" s="2"/>
       <c r="L23" s="2"/>
       <c r="M23" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="N23" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D24" s="1" t="n">
         <v>25</v>
@@ -1445,212 +1502,224 @@
       <c r="J24" s="2"/>
       <c r="K24" s="2"/>
       <c r="L24" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="M24" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="N24" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
+        <v>94</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D25" s="1" t="n">
+        <v>25</v>
+      </c>
       <c r="E25" s="2"/>
       <c r="F25" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G25" s="2"/>
       <c r="H25" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
       <c r="K25" s="2"/>
       <c r="L25" s="2"/>
       <c r="M25" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="N25" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
+        <v>97</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D26" s="1" t="n">
+        <v>25</v>
+      </c>
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
       <c r="G26" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I26" s="2"/>
       <c r="J26" s="2"/>
       <c r="K26" s="2"/>
       <c r="L26" s="2"/>
       <c r="M26" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="N26" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
+        <v>99</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D27" s="1" t="n">
+        <v>25</v>
+      </c>
       <c r="E27" s="2"/>
       <c r="F27" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G27" s="2"/>
       <c r="H27" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I27" s="2"/>
       <c r="J27" s="2"/>
       <c r="K27" s="2"/>
       <c r="L27" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="M27" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="N27" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D28" s="1" t="n">
         <v>25</v>
       </c>
       <c r="E28" s="2"/>
       <c r="F28" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H28" s="2"/>
       <c r="I28" s="2"/>
       <c r="J28" s="2"/>
       <c r="K28" s="2"/>
       <c r="L28" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="M28" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="N28" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D29" s="1" t="n">
         <v>30</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F29" s="2"/>
       <c r="G29" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H29" s="2"/>
       <c r="I29" s="2"/>
       <c r="J29" s="2"/>
       <c r="K29" s="2"/>
       <c r="L29" s="1" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="M29" s="1" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="N29" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E30" s="2"/>
       <c r="F30" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H30" s="2"/>
       <c r="I30" s="2"/>
       <c r="J30" s="2"/>
       <c r="K30" s="2"/>
       <c r="L30" s="1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="M30" s="1" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="N30" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D31" s="1" t="n">
         <v>30</v>
@@ -1663,109 +1732,123 @@
       <c r="J31" s="2"/>
       <c r="K31" s="2"/>
       <c r="L31" s="1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="M31" s="1" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="N31" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
+        <v>118</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D32" s="1" t="n">
+        <v>30</v>
+      </c>
       <c r="E32" s="2"/>
       <c r="F32" s="2"/>
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
       <c r="I32" s="2"/>
       <c r="J32" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="K32" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="L32" s="2"/>
       <c r="M32" s="1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="N32" s="1" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="C33" s="2"/>
-      <c r="D33" s="2"/>
+        <v>122</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D33" s="1" t="n">
+        <v>30</v>
+      </c>
       <c r="E33" s="2"/>
       <c r="F33" s="2"/>
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
       <c r="I33" s="2"/>
       <c r="J33" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="K33" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="L33" s="2"/>
       <c r="M33" s="1" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="N33" s="1" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="C34" s="2"/>
-      <c r="D34" s="2"/>
+        <v>66</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D34" s="1" t="n">
+        <v>30</v>
+      </c>
       <c r="E34" s="2"/>
       <c r="F34" s="2"/>
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
       <c r="I34" s="2"/>
       <c r="J34" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="K34" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="L34" s="2"/>
       <c r="M34" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="N34" s="1" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="C35" s="2"/>
+        <v>125</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>15</v>
+      </c>
       <c r="D35" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E35" s="2"/>
       <c r="F35" s="2"/>
@@ -1773,62 +1856,62 @@
       <c r="H35" s="2"/>
       <c r="I35" s="2"/>
       <c r="J35" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="K35" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="L35" s="2"/>
       <c r="M35" s="1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="N35" s="1" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D36" s="1" t="n">
         <v>30</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F36" s="2"/>
       <c r="G36" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H36" s="2"/>
       <c r="I36" s="2"/>
       <c r="J36" s="2"/>
       <c r="K36" s="2"/>
       <c r="L36" s="1" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="M36" s="1" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="N36" s="1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D37" s="1" t="n">
         <v>25</v>
@@ -1841,58 +1924,66 @@
       <c r="J37" s="2"/>
       <c r="K37" s="2"/>
       <c r="L37" s="1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="M37" s="1" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="N37" s="1" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="C38" s="2"/>
-      <c r="D38" s="2"/>
+        <v>135</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D38" s="1" t="n">
+        <v>25</v>
+      </c>
       <c r="E38" s="2"/>
       <c r="F38" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G38" s="2"/>
       <c r="H38" s="2"/>
       <c r="I38" s="2"/>
       <c r="J38" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="K38" s="2"/>
       <c r="L38" s="2"/>
       <c r="M38" s="1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="N38" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="C39" s="2"/>
-      <c r="D39" s="2"/>
+        <v>138</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D39" s="1" t="n">
+        <v>25</v>
+      </c>
       <c r="E39" s="2"/>
       <c r="F39" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H39" s="2"/>
       <c r="I39" s="2"/>
@@ -1900,49 +1991,53 @@
       <c r="K39" s="2"/>
       <c r="L39" s="2"/>
       <c r="M39" s="1" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="N39" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="C40" s="2"/>
-      <c r="D40" s="2"/>
+        <v>140</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D40" s="1" t="n">
+        <v>25</v>
+      </c>
       <c r="E40" s="2"/>
       <c r="F40" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G40" s="2"/>
       <c r="H40" s="2"/>
       <c r="I40" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J40" s="2"/>
       <c r="K40" s="2"/>
       <c r="L40" s="2"/>
       <c r="M40" s="1" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="N40" s="1" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D41" s="1" t="n">
         <v>30</v>
@@ -1950,33 +2045,33 @@
       <c r="E41" s="2"/>
       <c r="F41" s="2"/>
       <c r="G41" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H41" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I41" s="2"/>
       <c r="J41" s="2"/>
       <c r="K41" s="2"/>
       <c r="L41" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="M41" s="1" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="N41" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D42" s="1" t="n">
         <v>30</v>
@@ -1989,58 +2084,66 @@
       <c r="J42" s="2"/>
       <c r="K42" s="2"/>
       <c r="L42" s="1" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="M42" s="1" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="N42" s="1" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="C43" s="2"/>
-      <c r="D43" s="2"/>
+        <v>149</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D43" s="1" t="n">
+        <v>30</v>
+      </c>
       <c r="E43" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G43" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H43" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I43" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J43" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="K43" s="2"/>
       <c r="L43" s="2"/>
       <c r="M43" s="2"/>
       <c r="N43" s="1" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="C44" s="2"/>
-      <c r="D44" s="2"/>
+        <v>151</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D44" s="1" t="n">
+        <v>30</v>
+      </c>
       <c r="E44" s="2"/>
       <c r="F44" s="2"/>
       <c r="G44" s="2"/>
@@ -2048,66 +2151,66 @@
       <c r="I44" s="2"/>
       <c r="J44" s="2"/>
       <c r="K44" s="1" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="L44" s="2"/>
       <c r="M44" s="2"/>
       <c r="N44" s="1" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D45" s="1" t="n">
         <v>30</v>
       </c>
       <c r="E45" s="2"/>
       <c r="F45" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G45" s="2"/>
       <c r="H45" s="2"/>
       <c r="I45" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J45" s="2"/>
       <c r="K45" s="2"/>
       <c r="L45" s="1" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="M45" s="1" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="N45" s="1" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D46" s="1" t="n">
         <v>25</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G46" s="2"/>
       <c r="H46" s="2"/>
@@ -2115,36 +2218,36 @@
       <c r="J46" s="2"/>
       <c r="K46" s="2"/>
       <c r="L46" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="M46" s="1" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="N46" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>160</v>
+        <v>86</v>
       </c>
       <c r="E47" s="2"/>
       <c r="F47" s="2"/>
       <c r="G47" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H47" s="2"/>
       <c r="I47" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J47" s="2"/>
       <c r="K47" s="2"/>
@@ -2166,26 +2269,26 @@
         <v>164</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D48" s="1" t="n">
         <v>30</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F48" s="2"/>
       <c r="G48" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H48" s="3" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="I48" s="2"/>
       <c r="J48" s="2"/>
       <c r="K48" s="2"/>
       <c r="L48" s="1" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="M48" s="1" t="s">
         <v>165</v>
@@ -2202,20 +2305,20 @@
         <v>167</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D49" s="1" t="n">
         <v>30</v>
       </c>
       <c r="E49" s="2"/>
       <c r="F49" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G49" s="2"/>
       <c r="H49" s="2"/>
       <c r="I49" s="2"/>
       <c r="J49" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="K49" s="2"/>
       <c r="L49" s="1" t="s">
@@ -2236,7 +2339,7 @@
         <v>171</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D50" s="1" t="n">
         <v>30</v>
@@ -2265,15 +2368,19 @@
       <c r="B51" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="C51" s="2"/>
-      <c r="D51" s="2"/>
+      <c r="C51" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D51" s="1" t="n">
+        <v>30</v>
+      </c>
       <c r="E51" s="2"/>
       <c r="F51" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G51" s="2"/>
       <c r="H51" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I51" s="2"/>
       <c r="J51" s="2"/>
@@ -2291,17 +2398,21 @@
       <c r="B52" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="C52" s="2"/>
-      <c r="D52" s="2"/>
+      <c r="C52" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D52" s="1" t="n">
+        <v>30</v>
+      </c>
       <c r="E52" s="2"/>
       <c r="F52" s="2"/>
       <c r="G52" s="2"/>
       <c r="H52" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I52" s="2"/>
       <c r="J52" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="K52" s="2"/>
       <c r="L52" s="2"/>
@@ -2319,7 +2430,9 @@
       <c r="B53" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="C53" s="2"/>
+      <c r="C53" s="2" t="s">
+        <v>15</v>
+      </c>
       <c r="D53" s="1" t="s">
         <v>180</v>
       </c>
@@ -2327,11 +2440,11 @@
       <c r="F53" s="2"/>
       <c r="G53" s="2"/>
       <c r="H53" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I53" s="2"/>
       <c r="J53" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="K53" s="2"/>
       <c r="L53" s="2"/>
@@ -2349,17 +2462,21 @@
       <c r="B54" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="C54" s="2"/>
-      <c r="D54" s="2"/>
+      <c r="C54" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D54" s="1" t="n">
+        <v>30</v>
+      </c>
       <c r="E54" s="2"/>
       <c r="F54" s="2"/>
       <c r="G54" s="2"/>
       <c r="H54" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I54" s="2"/>
       <c r="J54" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="K54" s="2"/>
       <c r="L54" s="2"/>
@@ -2378,19 +2495,19 @@
         <v>184</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>185</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F55" s="2"/>
       <c r="G55" s="2"/>
       <c r="H55" s="2"/>
       <c r="I55" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J55" s="2"/>
       <c r="K55" s="2"/>
@@ -2412,26 +2529,26 @@
         <v>189</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>160</v>
+        <v>86</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F56" s="2"/>
       <c r="G56" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H56" s="2"/>
       <c r="I56" s="2"/>
       <c r="J56" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="K56" s="2"/>
       <c r="L56" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="M56" s="1" t="s">
         <v>190</v>
@@ -2448,7 +2565,7 @@
         <v>192</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D57" s="1" t="n">
         <v>30</v>
@@ -2457,11 +2574,11 @@
       <c r="F57" s="2"/>
       <c r="G57" s="2"/>
       <c r="H57" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I57" s="2"/>
       <c r="J57" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="K57" s="2"/>
       <c r="L57" s="1" t="s">

</xml_diff>